<commit_message>
Changes in name data
</commit_message>
<xml_diff>
--- a/src/main/resources/name_data.xlsx
+++ b/src/main/resources/name_data.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\91998\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\91998\Desktop\Amazon\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29FF0EA5-3F15-4FE3-B064-FE28D17F66F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF853CF1-042A-4002-BCE1-981EB4022762}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{6D32EFCC-109B-44EF-8674-EA9C70186219}"/>
+    <workbookView xWindow="2616" yWindow="2616" windowWidth="17280" windowHeight="8964" activeTab="3" xr2:uid="{6D32EFCC-109B-44EF-8674-EA9C70186219}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>username</t>
   </si>
@@ -78,6 +79,9 @@
   </si>
   <si>
     <t>manikgupta54@yahoo.com</t>
+  </si>
+  <si>
+    <t>data`</t>
   </si>
 </sst>
 </file>
@@ -536,7 +540,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C32764C0-4A62-46AC-92B7-6DB75F6064E5}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:A3"/>
     </sheetView>
   </sheetViews>
@@ -564,4 +568,35 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F445E7CA-74E3-4D05-B8C1-6C0D5564F367}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>